<commit_message>
add model to tg
- so baaaad.....
</commit_message>
<xml_diff>
--- a/text_model/text_analysis_result.xlsx
+++ b/text_model/text_analysis_result.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,7 +466,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Нет, хуйня это ваш зумерский снюс.</t>
+          <t xml:space="preserve">Нет, хуйня это ваш зумерский снюс. </t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -494,8 +494,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t xml:space="preserve">
- Всем привет, как дела?</t>
+          <t xml:space="preserve"> Всем привет, как дела? </t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -523,29 +522,81 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t xml:space="preserve">
- (⌒▽⌒)☆【B】ШｋＯЛｅ≧◡≦Tak匚【k】ㄚЧH̲o̲＼(￣▽￣)／ 
- ║ [ Н҉А҉ С҉Л҉У҉Ч҉А҉Й҉ Е҉С҉Л҉И҉ Я҉ У҉М҉Р҉У 
- Группа создана в экспериментальных целях 
- Как настоящий ру$$кий я предпочту убойный насвай, синтетический гашиш, метадон, и мефедрон</t>
+          <t xml:space="preserve">  ║ [ Н҉А҉ С҉Л҉У҉Ч҉А҉Й҉ Е҉С҉Л҉И҉ Я҉ У҉М҉Р҉У.  </t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>⌒▽⌒ ☆【b】шｋｏлｅ≧◡≦tak匚【k】ㄚчh̲o̲＼ ￣▽￣ ／ ║ н҉а҉ с҉л҉у҉ч҉а҉й҉ е҉с҉л҉и҉ я҉ у҉м҉р҉у группа создана в экспериментальных целях как настоящий ру кий я предпочту убойный насвай синтетический гашиш метадон и мефедрон</t>
+          <t>║ н҉а҉ с҉л҉у҉ч҉а҉й҉ е҉с҉л҉и҉ я҉ у҉м҉р҉у</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>⌒▽⌒ ☆【b】шｋｏлｅ≧◡≦tak匚【k】ㄚчh̲o̲＼ ￣▽￣ ／ ║ н҉а҉ с҉л҉у҉ч҉а҉й҉ е҉с҉л҉и҉ я҉ у҉м҉р҉ группа создать в экспериментальный цель как настоящий ру кий я предпочесть убойный насвая синтетический гашиш метадон и мефедрон</t>
+          <t>║ н҉а҉ с҉л҉у҉ч҉а҉й҉ е҉с҉л҉и҉ я҉ у҉м҉р҉</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>⌒▽⌒ ☆【b】шｋｏлｅ≧◡≦tak匚【k】ㄚчh̲o̲＼ ￣▽￣ ／ ║ н҉а҉ с҉л҉у҉ч҉а҉й҉ е҉с҉л҉и҉ я҉ у҉м҉р҉ группа создать экспериментальный цель настоящий ру кий предпочесть убойный насвая синтетический гашиш метадон мефедрон</t>
+          <t>║ н҉а҉ с҉л҉у҉ч҉а҉й҉ е҉с҉л҉и҉ я҉ у҉м҉р҉</t>
         </is>
       </c>
       <c r="F4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Группа создана в экспериментальных целях </t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>группа создана в экспериментальных целях</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>группа создать в экспериментальный цель</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>группа создать экспериментальный цель</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Как настоящий ру$$кий я предпочту убойный насвай, синтетический гашиш, метадон, и мефедрон</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>как настоящий ру кий я предпочту убойный насвай синтетический гашиш метадон и мефедрон</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>как настоящий ру кий я предпочесть убойный насвая синтетический гашиш метадон и мефедрон</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>настоящий ру кий предпочесть убойный насвая синтетический гашиш метадон мефедрон</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>